<commit_message>
Update GUI Twitter, Website
</commit_message>
<xml_diff>
--- a/data/tweets/#DREAMCATCHER/#DREAMCATCHER_11042022.xlsx
+++ b/data/tweets/#DREAMCATCHER/#DREAMCATCHER_11042022.xlsx
@@ -492,27 +492,27 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>dcatcherbr</t>
+          <t>moramourlila</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Desde 05/12/2016</t>
+          <t>warm, cozy hobbit-hole, Shire</t>
         </is>
       </c>
       <c r="D2" s="2" t="n">
-        <v>44662.1366550926</v>
+        <v>44662.91146990741</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>l INSTAGRAM Atualizao da SuA no story sualelbora PiscandoDreamcatcher</t>
+          <t>Siyeon from Dreamcatcher is so dangerous</t>
         </is>
       </c>
       <c r="F2" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H2" t="inlineStr">
         <is>
@@ -521,7 +521,7 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>https://twitter.com/twitter/statuses/1513249655475351553</t>
+          <t>https://twitter.com/twitter/statuses/1513530438702141446</t>
         </is>
       </c>
     </row>
@@ -533,36 +533,36 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>deukaenthusiast</t>
+          <t>bloodyponey</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>☣☠☣</t>
+          <t>21, she/her</t>
         </is>
       </c>
       <c r="D3" s="2" t="n">
-        <v>44662.13214120371</v>
+        <v>44662.91065972222</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>my friends just bullied me for being active on twitter Im sorry that I have an important comeback to promote lmao</t>
+          <t>N O PREDIO DA DCC DreamcatcherndAlbum Apocalypse Saveus MAISON</t>
         </is>
       </c>
       <c r="F3" t="n">
         <v>0</v>
       </c>
       <c r="G3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>positive</t>
+          <t>neutral</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>https://twitter.com/twitter/statuses/1513248020896305155</t>
+          <t>https://twitter.com/twitter/statuses/1513530144685707265</t>
         </is>
       </c>
     </row>
@@ -574,27 +574,27 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>deukaemobile</t>
+          <t>suayeonarchives</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>don't repost/claim as yours</t>
+          <t>suayeontonie</t>
         </is>
       </c>
       <c r="D4" s="2" t="n">
-        <v>44662.12982638889</v>
+        <v>44662.91043981481</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Maison 'MV Teaser' Desktop version hfdreamcatcher Dreamcatcher ApocalypseSaveus MAISON</t>
+          <t>Dreamcatcher videos MMT Dreamcatcher suayeon</t>
         </is>
       </c>
       <c r="F4" t="n">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="G4" t="n">
-        <v>63</v>
+        <v>1</v>
       </c>
       <c r="H4" t="inlineStr">
         <is>
@@ -603,7 +603,7 @@
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>https://twitter.com/twitter/statuses/1513247181184114693</t>
+          <t>https://twitter.com/twitter/statuses/1513530065010626560</t>
         </is>
       </c>
     </row>
@@ -615,36 +615,36 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>yoohki_</t>
+          <t>Gombers04</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>she they # lesbian # 17</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="D5" s="2" t="n">
-        <v>44662.1271412037</v>
+        <v>44662.90935185185</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Dreamcatcher Heardle 15 Dreamcatcher2ndAlbumApocalypse SaveusDreamcatcherComeback</t>
+          <t>In just under 19 hours Ill be listening to an all new Dreamcatcher album were really almost here guys</t>
         </is>
       </c>
       <c r="F5" t="n">
         <v>0</v>
       </c>
       <c r="G5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>neutral</t>
+          <t>positive</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>https://twitter.com/twitter/statuses/1513246208814243842</t>
+          <t>https://twitter.com/twitter/statuses/1513529670964183044</t>
         </is>
       </c>
     </row>
@@ -656,27 +656,27 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>YoohyeonHourly</t>
+          <t>bloodyponey</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>unknown</t>
+          <t>21, she/her</t>
         </is>
       </c>
       <c r="D6" s="2" t="n">
-        <v>44662.125</v>
+        <v>44662.90931712963</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Dreamcatcher YOOHYEON hfdreamcatcher</t>
+          <t>COMO CONSEGUIRAM SUBIR AQUI PRA PICHAR DreamcatcherndAlbum Apocalypse Saveus</t>
         </is>
       </c>
       <c r="F6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G6" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="H6" t="inlineStr">
         <is>
@@ -685,7 +685,7 @@
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>https://twitter.com/twitter/statuses/1513245432696086531</t>
+          <t>https://twitter.com/twitter/statuses/1513529660994465793</t>
         </is>
       </c>
     </row>
@@ -697,7 +697,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>gahjidongfiles</t>
+          <t>0000kai000</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -706,18 +706,18 @@
         </is>
       </c>
       <c r="D7" s="2" t="n">
-        <v>44662.12335648148</v>
+        <v>44662.90928240741</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Tracks 8 11 amp 14 GAHYEON JIU HANDONG Dreamcatcher</t>
+          <t>foryoohyeon Am looking forward to all the performances Cant wait to see the choreo for Maison and also locked</t>
         </is>
       </c>
       <c r="F7" t="n">
         <v>0</v>
       </c>
       <c r="G7" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="H7" t="inlineStr">
         <is>
@@ -726,7 +726,7 @@
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>https://twitter.com/twitter/statuses/1513244838350761991</t>
+          <t>https://twitter.com/twitter/statuses/1513529647111180290</t>
         </is>
       </c>
     </row>
@@ -738,27 +738,27 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>dcatcherbr</t>
+          <t>bloodyponey</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Desde 05/12/2016</t>
+          <t>21, she/her</t>
         </is>
       </c>
       <c r="D8" s="2" t="n">
-        <v>44662.12292824074</v>
+        <v>44662.90891203703</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>l INSTAGRAM Comentrios da JiU e Handong Eu estou bem KekekekekekeDreamcatcher</t>
+          <t>GOSTEI DO CENARIO TA PARECENDO A CIDADE DE ONE PUNCH MAN DreamcatcherndAlbum Apocalypse Saveus</t>
         </is>
       </c>
       <c r="F8" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G8" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="H8" t="inlineStr">
         <is>
@@ -767,7 +767,7 @@
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>https://twitter.com/twitter/statuses/1513244680053526533</t>
+          <t>https://twitter.com/twitter/statuses/1513529514244161538</t>
         </is>
       </c>
     </row>
@@ -779,20 +779,20 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>YouthOfMaes</t>
+          <t>fabio_carassa</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>unknown</t>
+          <t>Vigo, España</t>
         </is>
       </c>
       <c r="D9" s="2" t="n">
-        <v>44662.11755787037</v>
+        <v>44662.90887731482</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>DREAMCATCHER 2nd Album Apocalypse Save us PreOrder MeetampCall Event</t>
+          <t>DeuKaeRadio TonyAguilarOfi Los GlobalShow hfdreamcatcher Deseamos que se reproduzca MAISON de las reinas</t>
         </is>
       </c>
       <c r="F9" t="n">
@@ -808,7 +808,7 @@
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>https://twitter.com/twitter/statuses/1513242735545044992</t>
+          <t>https://twitter.com/twitter/statuses/1513529501510160384</t>
         </is>
       </c>
     </row>
@@ -820,7 +820,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>yearlydeukae</t>
+          <t>mik_silv</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -829,18 +829,18 @@
         </is>
       </c>
       <c r="D10" s="2" t="n">
-        <v>44662.11458333334</v>
+        <v>44662.90858796296</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Dreamcatcher YOOHYEON hfdreamcatcher</t>
+          <t>LuvDeukae DIAS PARA O APOCALYPSEDreamcatcher hfdreamcatcher</t>
         </is>
       </c>
       <c r="F10" t="n">
         <v>0</v>
       </c>
       <c r="G10" t="n">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="H10" t="inlineStr">
         <is>
@@ -849,7 +849,7 @@
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>https://twitter.com/twitter/statuses/1513241656597880839</t>
+          <t>https://twitter.com/twitter/statuses/1513529395767492610</t>
         </is>
       </c>
     </row>
@@ -861,27 +861,27 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>deukaeKdata</t>
+          <t>bloodyponey</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>unknown</t>
+          <t>21, she/her</t>
         </is>
       </c>
       <c r="D11" s="2" t="n">
-        <v>44662.11241898148</v>
+        <v>44662.90825231482</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Apocalypse Save Us preorders on Ktown4u have now surpassed those of Summer Holiday Dreamcatcher hfdreamcatcher</t>
+          <t>MULHER AGR Q TE VI ME PERDOA DreamcatcherndAlbum Apocalypse Saveus MAISON</t>
         </is>
       </c>
       <c r="F11" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="G11" t="n">
-        <v>113</v>
+        <v>0</v>
       </c>
       <c r="H11" t="inlineStr">
         <is>
@@ -890,7 +890,7 @@
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>https://twitter.com/twitter/statuses/1513240873202561036</t>
+          <t>https://twitter.com/twitter/statuses/1513529273780482056</t>
         </is>
       </c>
     </row>
@@ -902,27 +902,27 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>dcatcherbr</t>
+          <t>flowearb</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Desde 05/12/2016</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="D12" s="2" t="n">
-        <v>44662.11231481482</v>
+        <v>44662.90782407407</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>l VIDEO JiU com Somnias diante da rdio Young Street Ela olhando e acenando para os fs mesm</t>
+          <t>JIU Dreamcatcher</t>
         </is>
       </c>
       <c r="F12" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G12" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="H12" t="inlineStr">
         <is>
@@ -931,7 +931,7 @@
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>https://twitter.com/twitter/statuses/1513240835978055690</t>
+          <t>https://twitter.com/twitter/statuses/1513529116607365136</t>
         </is>
       </c>
     </row>
@@ -943,27 +943,27 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>utopiasua</t>
+          <t>bloodyponey</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t xml:space="preserve">22 she/her </t>
+          <t>21, she/her</t>
         </is>
       </c>
       <c r="D13" s="2" t="n">
-        <v>44662.10915509259</v>
+        <v>44662.90752314815</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Dreamcatcher Heardle 15 Dreamcatcher2ndAlbumApocalypse SaveusDreamcatcherComeback</t>
+          <t>GAHYEON PARECE UM ANO DreamcatcherndAlbum Apocalypse Saveus MAISON</t>
         </is>
       </c>
       <c r="F13" t="n">
         <v>0</v>
       </c>
       <c r="G13" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H13" t="inlineStr">
         <is>
@@ -972,7 +972,7 @@
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>https://twitter.com/twitter/statuses/1513239689586786306</t>
+          <t>https://twitter.com/twitter/statuses/1513529011397345288</t>
         </is>
       </c>
     </row>
@@ -984,20 +984,20 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>SINGNlE</t>
+          <t>ChourakiMlusin1</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>dc pk wjsn • priv @ireheeks</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="D14" s="2" t="n">
-        <v>44662.10747685185</v>
+        <v>44662.90722222222</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Dreamcatcher Heardle 15 Dreamcatcher2ndAlbumApocalypse SaveusDreamcatcherComeback</t>
+          <t>Merci Puffygator pour cette magnifique illustration reprsentant Lewis un bassaris Ce petit animal est la mas</t>
         </is>
       </c>
       <c r="F14" t="n">
@@ -1013,7 +1013,7 @@
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>https://twitter.com/twitter/statuses/1513239080494149635</t>
+          <t>https://twitter.com/twitter/statuses/1513528900856520705</t>
         </is>
       </c>
     </row>
@@ -1025,27 +1025,27 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>_7spirits</t>
+          <t>flowearb</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t xml:space="preserve">썸냐 1기 </t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="D15" s="2" t="n">
-        <v>44662.10688657407</v>
+        <v>44662.90641203704</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>asianjunkiecom Thank you for the GADreamcatcher ApocalypseSaveUs ApocalypseSaveus</t>
+          <t>Dreamcatcher</t>
         </is>
       </c>
       <c r="F15" t="n">
         <v>0</v>
       </c>
       <c r="G15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H15" t="inlineStr">
         <is>
@@ -1054,7 +1054,7 @@
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>https://twitter.com/twitter/statuses/1513238866358161413</t>
+          <t>https://twitter.com/twitter/statuses/1513528605044838407</t>
         </is>
       </c>
     </row>
@@ -1066,7 +1066,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>singjiarchive</t>
+          <t>yearlydeukae</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -1075,18 +1075,18 @@
         </is>
       </c>
       <c r="D16" s="2" t="n">
-        <v>44662.10636574074</v>
+        <v>44662.90625</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>Dreamcatcher JIU SIYEON</t>
+          <t>Dreamcatcher YOOHYEON hfdreamcatcher</t>
         </is>
       </c>
       <c r="F16" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G16" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="H16" t="inlineStr">
         <is>
@@ -1095,7 +1095,7 @@
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>https://twitter.com/twitter/statuses/1513238679598338055</t>
+          <t>https://twitter.com/twitter/statuses/1513528546941030403</t>
         </is>
       </c>
     </row>
@@ -1107,20 +1107,20 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>kimsnaps</t>
+          <t>bloodyponey</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Venezuela</t>
+          <t>21, she/her</t>
         </is>
       </c>
       <c r="D17" s="2" t="n">
-        <v>44662.10466435185</v>
+        <v>44662.90579861111</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>DREAMCATCHER 'Weekly Idol' EP Reaction via YouTube Dreamcatcher hfdreamcatcher</t>
+          <t>DreamcatcherndAlbum Apocalypse Saveus MAISON E OQ ISSO NAS MOS JUTSU KATON</t>
         </is>
       </c>
       <c r="F17" t="n">
@@ -1136,7 +1136,7 @@
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>https://twitter.com/twitter/statuses/1513238062968578050</t>
+          <t>https://twitter.com/twitter/statuses/1513528384801939468</t>
         </is>
       </c>
     </row>
@@ -1148,20 +1148,20 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>_7spirits</t>
+          <t>i6_yubin</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t xml:space="preserve">썸냐 1기 </t>
+          <t xml:space="preserve">( . ) read the carrd 💭_ </t>
         </is>
       </c>
       <c r="D18" s="2" t="n">
-        <v>44662.10452546296</v>
+        <v>44662.90518518518</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>symylife Thank you for the ga I would really like to have A version14SongsOfTheApocalypse</t>
+          <t>pkjvcut DIAS PARA O APOCALYPSEDreamcatcher hfdreamcatcher</t>
         </is>
       </c>
       <c r="F18" t="n">
@@ -1177,7 +1177,7 @@
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>https://twitter.com/twitter/statuses/1513238013190496257</t>
+          <t>https://twitter.com/twitter/statuses/1513528161040015366</t>
         </is>
       </c>
     </row>
@@ -1189,20 +1189,20 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>TuaTeratas</t>
+          <t>bloodyponey</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Selangor, Malaysia</t>
+          <t>21, she/her</t>
         </is>
       </c>
       <c r="D19" s="2" t="n">
-        <v>44662.10321759259</v>
+        <v>44662.90450231481</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>to be but Im cautiously optimistic Dreamcatcher 2ndAlbum Apocalypse Saveus MAISON</t>
+          <t>DAMI FODONA DreamcatcherndAlbum Apocalypse Saveus MAISON</t>
         </is>
       </c>
       <c r="F19" t="n">
@@ -1218,7 +1218,7 @@
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>https://twitter.com/twitter/statuses/1513237540467527683</t>
+          <t>https://twitter.com/twitter/statuses/1513527915459317767</t>
         </is>
       </c>
     </row>
@@ -1230,20 +1230,20 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>eclipsetzy</t>
+          <t>Leanne45671141</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>20 she/her | black | -15 dnf</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="D20" s="2" t="n">
-        <v>44662.10106481481</v>
+        <v>44662.90432870371</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>Dreamcatcher Heardle 15 Dreamcatcher2ndAlbumApocalypse SaveusDreamcatcherComeback</t>
+          <t>LuvDeukae DIAS PARA O APOCALYPSEDreamcatcher hfdreamcatcher</t>
         </is>
       </c>
       <c r="F20" t="n">
@@ -1259,7 +1259,7 @@
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>https://twitter.com/twitter/statuses/1513236756795207682</t>
+          <t>https://twitter.com/twitter/statuses/1513527853614309383</t>
         </is>
       </c>
     </row>
@@ -1271,20 +1271,20 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>jiumoradita</t>
+          <t>dreamer_atzdc</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>unknown</t>
+          <t>*.☆ Nightmare City ☆.*</t>
         </is>
       </c>
       <c r="D21" s="2" t="n">
-        <v>44662.09744212963</v>
+        <v>44662.90400462963</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>LVale0703 jellyvotesph done for Dreamcatcher</t>
+          <t>en minutos es el DDay para el comeback AYUDA Dreamcatcher ndAlbum Apocalypse Saveus MAISON</t>
         </is>
       </c>
       <c r="F21" t="n">
@@ -1300,7 +1300,7 @@
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>https://twitter.com/twitter/statuses/1513235444091269122</t>
+          <t>https://twitter.com/twitter/statuses/1513527734072483842</t>
         </is>
       </c>
     </row>
@@ -1312,36 +1312,36 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>dcatcherbr</t>
+          <t>CHERRYBYULIE</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Desde 05/12/2016</t>
+          <t>she | her • 21</t>
         </is>
       </c>
       <c r="D22" s="2" t="n">
-        <v>44662.09354166667</v>
+        <v>44662.9025462963</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>1004 l INFO O mv de Endless Night ultrapassou 100 mil likes no YouTubeDreamcatcher</t>
+          <t>I cannot wait to see the Dreamcatcher photocards this time around ApocalypseSaveUs Dreamcatcher</t>
         </is>
       </c>
       <c r="F22" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G22" t="n">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>negative</t>
+          <t>neutral</t>
         </is>
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>https://twitter.com/twitter/statuses/1513234032464695296</t>
+          <t>https://twitter.com/twitter/statuses/1513527206374346754</t>
         </is>
       </c>
     </row>
@@ -1353,27 +1353,27 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>_sspag</t>
+          <t>bloodyponey</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>unknown</t>
+          <t>21, she/her</t>
         </is>
       </c>
       <c r="D23" s="2" t="n">
-        <v>44662.09214120371</v>
+        <v>44662.90211805556</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>Obligatory Sua drawing after Siyeon's Dreamcatcher Dreamcatcherfanart ApocalypseSaveUs SuA</t>
+          <t>minji n tenho oq falar simplesmente me agrada em todos os lados quando a questo moda essa mulher deveria ser e</t>
         </is>
       </c>
       <c r="F23" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G23" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="H23" t="inlineStr">
         <is>
@@ -1382,7 +1382,7 @@
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>https://twitter.com/twitter/statuses/1513233525692153860</t>
+          <t>https://twitter.com/twitter/statuses/1513527050430205960</t>
         </is>
       </c>
     </row>
@@ -1394,20 +1394,20 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>yoohyncrush</t>
+          <t>Matias10Rain</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t xml:space="preserve">Grand line </t>
+          <t>Orlando, Florida.</t>
         </is>
       </c>
       <c r="D24" s="2" t="n">
-        <v>44662.09204861111</v>
+        <v>44662.901875</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>Dreamcatcher hala hala dance cover all members focusDreamcatcher hfdreamcatcher</t>
+          <t>I got mine 1 week ago I hope can see something before Bloodwork Dreamcatcher DreamcatcherComeback</t>
         </is>
       </c>
       <c r="F24" t="n">
@@ -1423,7 +1423,7 @@
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>https://twitter.com/twitter/statuses/1513233489755267077</t>
+          <t>https://twitter.com/twitter/statuses/1513526963146797071</t>
         </is>
       </c>
     </row>
@@ -1435,20 +1435,20 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>sannakore</t>
+          <t>LittlePureHeart</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>The Dreamworld</t>
+          <t>Destiny Island 🏝</t>
         </is>
       </c>
       <c r="D25" s="2" t="n">
-        <v>44662.08765046296</v>
+        <v>44662.90186342593</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>Congratz to Gahyeon Good job InsomniaDreamcatcher hfdreamcatcher</t>
+          <t>PaniclnTheCity hfdreamcatcher Thank you for the GA Dreamcatcher ApocalypseSaveus</t>
         </is>
       </c>
       <c r="F25" t="n">
@@ -1459,12 +1459,12 @@
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>positive</t>
+          <t>neutral</t>
         </is>
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>https://twitter.com/twitter/statuses/1513231896775430148</t>
+          <t>https://twitter.com/twitter/statuses/1513526957497262086</t>
         </is>
       </c>
     </row>
@@ -1476,20 +1476,20 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>imnikky</t>
+          <t>bloodyponey</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Los Angeles, CA</t>
+          <t>21, she/her</t>
         </is>
       </c>
       <c r="D26" s="2" t="n">
-        <v>44662.08667824074</v>
+        <v>44662.90121527778</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>Dreamcatcher Heardle 15 Dreamcatcher2ndAlbumApocalypse SaveusDreamcatcherComeback</t>
+          <t>CORRENTINHA DA BORA CUTI CUTI DreamcatcherndAlbum Apocalypse Saveus MAISON</t>
         </is>
       </c>
       <c r="F26" t="n">
@@ -1505,7 +1505,7 @@
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>https://twitter.com/twitter/statuses/1513231545774972929</t>
+          <t>https://twitter.com/twitter/statuses/1513526725556244482</t>
         </is>
       </c>
     </row>
@@ -1517,20 +1517,20 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>npqace</t>
+          <t>bloodyponey</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>he/him ⚧️</t>
+          <t>21, she/her</t>
         </is>
       </c>
       <c r="D27" s="2" t="n">
-        <v>44662.08658564815</v>
+        <v>44662.90074074074</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>LVale0703 jellyvotesph DoneDreamcatcher</t>
+          <t>APOSTO Q ESSA ROUPA DA YOOH IA ATE O CHAO MAS TIVERAM Q CORTAR PRA N CHAMAR OS BOMBEIROS Dreamcatcher</t>
         </is>
       </c>
       <c r="F27" t="n">
@@ -1546,7 +1546,7 @@
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>https://twitter.com/twitter/statuses/1513231510534602760</t>
+          <t>https://twitter.com/twitter/statuses/1513526551295447042</t>
         </is>
       </c>
     </row>
@@ -1558,27 +1558,27 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>yubinsblaze</t>
+          <t>4d_yangdam</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>a♡</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="D28" s="2" t="n">
-        <v>44662.08583333333</v>
+        <v>44662.90072916666</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>i was planning to plant seeds this week too tuesday it is ill get more tuesday or wednesday too</t>
+          <t>PaniclnTheCity hfdreamcatcher Thank you for this giveaway Dreamcatcher ApocalypseSaveUs MAISON</t>
         </is>
       </c>
       <c r="F28" t="n">
         <v>0</v>
       </c>
       <c r="G28" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H28" t="inlineStr">
         <is>
@@ -1587,7 +1587,7 @@
       </c>
       <c r="I28" t="inlineStr">
         <is>
-          <t>https://twitter.com/twitter/statuses/1513231237141442571</t>
+          <t>https://twitter.com/twitter/statuses/1513526547726344202</t>
         </is>
       </c>
     </row>
@@ -1599,20 +1599,20 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>InSomnias_alarm</t>
+          <t>ryujinfp</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t xml:space="preserve">فعلوا جرس التنبيهات 🔔 </t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="D29" s="2" t="n">
-        <v>44662.08340277777</v>
+        <v>44662.90046296296</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>Mwave Whosfan</t>
+          <t>PaniclnTheCity hfdreamcatcher Thank you so much for the ga hfdreamcatcher 2ndAlbum ApocalypseSaveUs Dreamcatcher</t>
         </is>
       </c>
       <c r="F29" t="n">
@@ -1623,12 +1623,12 @@
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>neutral</t>
+          <t>positive</t>
         </is>
       </c>
       <c r="I29" t="inlineStr">
         <is>
-          <t>https://twitter.com/twitter/statuses/1513230356115251212</t>
+          <t>https://twitter.com/twitter/statuses/1513526449927761920</t>
         </is>
       </c>
     </row>
@@ -1640,27 +1640,27 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>YoohyeonHourly</t>
+          <t>Dystopia_zip</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>unknown</t>
+          <t>Alone in the City</t>
         </is>
       </c>
       <c r="D30" s="2" t="n">
-        <v>44662.08334490741</v>
+        <v>44662.90033564815</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>Dreamcatcher YOOHYEON hfdreamcatcher</t>
+          <t>Like this tweet if you preordered hfdreamcatcher A SU on a website OTHER THAN ktown4u Im checking something</t>
         </is>
       </c>
       <c r="F30" t="n">
         <v>0</v>
       </c>
       <c r="G30" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H30" t="inlineStr">
         <is>
@@ -1669,7 +1669,7 @@
       </c>
       <c r="I30" t="inlineStr">
         <is>
-          <t>https://twitter.com/twitter/statuses/1513230336045596682</t>
+          <t>https://twitter.com/twitter/statuses/1513526405019144194</t>
         </is>
       </c>
     </row>
@@ -1681,36 +1681,36 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>deukaebrandr</t>
+          <t>roseftwheein</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>— 🔔⠀</t>
+          <t>Argentina</t>
         </is>
       </c>
       <c r="D31" s="2" t="n">
-        <v>44662.08163194444</v>
+        <v>44662.90001157407</v>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>Girl Group Brand Reputation Ranking for March 202227 DREAMCATCHER 2 Dreamcatcher</t>
+          <t>PSBuenosAires Espero ver a estas reinas en el lineup Dreamcatcher ndAlbum Apocalypse Saveus</t>
         </is>
       </c>
       <c r="F31" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G31" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>negative</t>
+          <t>neutral</t>
         </is>
       </c>
       <c r="I31" t="inlineStr">
         <is>
-          <t>https://twitter.com/twitter/statuses/1513229716240707590</t>
+          <t>https://twitter.com/twitter/statuses/1513526286248992771</t>
         </is>
       </c>
     </row>
@@ -1722,20 +1722,20 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>SuBulut_</t>
+          <t>bloodyponey</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>unknown</t>
+          <t>21, she/her</t>
         </is>
       </c>
       <c r="D32" s="2" t="n">
-        <v>44662.07991898148</v>
+        <v>44662.89972222222</v>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>LVale jellyvotesph Dreamcatcher ApocalypseSaveus ApocalypseSaveUsApocalypseSaveUs</t>
+          <t>A ROUPA DA SISI DreamcatcherndAlbum Apocalypse Saveus MAISON</t>
         </is>
       </c>
       <c r="F32" t="n">
@@ -1751,7 +1751,7 @@
       </c>
       <c r="I32" t="inlineStr">
         <is>
-          <t>https://twitter.com/twitter/statuses/1513229096272203781</t>
+          <t>https://twitter.com/twitter/statuses/1513526184046383104</t>
         </is>
       </c>
     </row>
@@ -1763,27 +1763,27 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>dcatcherbr</t>
+          <t>Matias10Rain</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Desde 05/12/2016</t>
+          <t>Orlando, Florida.</t>
         </is>
       </c>
       <c r="D33" s="2" t="n">
-        <v>44662.07878472222</v>
+        <v>44662.89946759259</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>l INSTAGRAM Atualizao da SuA no story sualelbora Clima agradvelDreamcatcher</t>
+          <t>I still havent bought AVE albums yet But waiting for the S version from hello82official Please do buy more if</t>
         </is>
       </c>
       <c r="F33" t="n">
         <v>2</v>
       </c>
       <c r="G33" t="n">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="H33" t="inlineStr">
         <is>
@@ -1792,7 +1792,7 @@
       </c>
       <c r="I33" t="inlineStr">
         <is>
-          <t>https://twitter.com/twitter/statuses/1513228686463492100</t>
+          <t>https://twitter.com/twitter/statuses/1513526091444625418</t>
         </is>
       </c>
     </row>
@@ -1804,20 +1804,20 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>braceletsanchan</t>
+          <t>bloodyponey</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Germany</t>
+          <t>21, she/her</t>
         </is>
       </c>
       <c r="D34" s="2" t="n">
-        <v>44662.07650462963</v>
+        <v>44662.89921296296</v>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>To everyone thats going to KPOPFlexI have some goodie bundles for preorderIf youre interested follow the in</t>
+          <t>lembrei das referencias q e elas tavam fazendo com arminhas no dedo DreamcatcherndAlbum Apocalypse Saveus MAISON</t>
         </is>
       </c>
       <c r="F34" t="n">
@@ -1833,7 +1833,7 @@
       </c>
       <c r="I34" t="inlineStr">
         <is>
-          <t>https://twitter.com/twitter/statuses/1513227859434872835</t>
+          <t>https://twitter.com/twitter/statuses/1513525997135708162</t>
         </is>
       </c>
     </row>
@@ -1845,36 +1845,36 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>InSomnias_alarm</t>
+          <t>fairydkyeom</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t xml:space="preserve">فعلوا جرس التنبيهات 🔔 </t>
+          <t xml:space="preserve">19 (she/her) </t>
         </is>
       </c>
       <c r="D35" s="2" t="n">
-        <v>44662.07483796297</v>
+        <v>44662.89905092592</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>hfdreamcatcher</t>
+          <t>okay but the choreography is so cool Im addicted to itApocalypseSaveUs Dreamcatcher hfdreamcatcher</t>
         </is>
       </c>
       <c r="F35" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G35" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>neutral</t>
+          <t>positive</t>
         </is>
       </c>
       <c r="I35" t="inlineStr">
         <is>
-          <t>https://twitter.com/twitter/statuses/1513227253135687684</t>
+          <t>https://twitter.com/twitter/statuses/1513525937274769411</t>
         </is>
       </c>
     </row>
@@ -1886,36 +1886,36 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>yearlydeukae</t>
+          <t>natashasofiam</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>unknown</t>
+          <t>Tompaso, Indonesia</t>
         </is>
       </c>
       <c r="D36" s="2" t="n">
-        <v>44662.07291666666</v>
+        <v>44662.89873842592</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>Dreamcatcher hfdreamcatcher</t>
+          <t>PaniclnTheCity LuminaBlackswan hfdreamcatcher Thankyou so much Thank you for the GAhfdreamcatcher</t>
         </is>
       </c>
       <c r="F36" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G36" t="n">
-        <v>29</v>
+        <v>0</v>
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>neutral</t>
+          <t>positive</t>
         </is>
       </c>
       <c r="I36" t="inlineStr">
         <is>
-          <t>https://twitter.com/twitter/statuses/1513226556998443010</t>
+          <t>https://twitter.com/twitter/statuses/1513525827333668868</t>
         </is>
       </c>
     </row>
@@ -1927,27 +1927,27 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>InSomnia_CTG</t>
+          <t>bloodyponey</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Cartagena, Colombia</t>
+          <t>21, she/her</t>
         </is>
       </c>
       <c r="D37" s="2" t="n">
-        <v>44662.07125</v>
+        <v>44662.89873842592</v>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>SiYeon Es primavera Trans ES InSomniaCTG Dreamcatcher</t>
+          <t>gostei das arminha ksdjakdjkajdkasdjkadjadjkasj DreamcatcherndAlbum Apocalypse Saveus MAISON</t>
         </is>
       </c>
       <c r="F37" t="n">
         <v>0</v>
       </c>
       <c r="G37" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H37" t="inlineStr">
         <is>
@@ -1956,7 +1956,7 @@
       </c>
       <c r="I37" t="inlineStr">
         <is>
-          <t>https://twitter.com/twitter/statuses/1513225955929698306</t>
+          <t>https://twitter.com/twitter/statuses/1513525825345306624</t>
         </is>
       </c>
     </row>
@@ -1968,27 +1968,27 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>takapanda_WithU</t>
+          <t>uwu_555</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>unknown</t>
+          <t>Somewhere in 2D World</t>
         </is>
       </c>
       <c r="D38" s="2" t="n">
-        <v>44662.06956018518</v>
+        <v>44662.89829861111</v>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>DreamcatcherApocalypse Saveus MAISON SUA</t>
+          <t>One For Deukae Now its your turn our wish is your wish Now go save the world dreamcatcher Maison</t>
         </is>
       </c>
       <c r="F38" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G38" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H38" t="inlineStr">
         <is>
@@ -1997,7 +1997,7 @@
       </c>
       <c r="I38" t="inlineStr">
         <is>
-          <t>https://twitter.com/twitter/statuses/1513225340176728064</t>
+          <t>https://twitter.com/twitter/statuses/1513525667987857408</t>
         </is>
       </c>
     </row>
@@ -2009,27 +2009,27 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>dcatcherbr</t>
+          <t>7flowers0fLight</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Desde 05/12/2016</t>
+          <t xml:space="preserve">En el Hoyuelo de Namjoon </t>
         </is>
       </c>
       <c r="D39" s="2" t="n">
-        <v>44662.06802083334</v>
+        <v>44662.89780092592</v>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>l WEVERSE Comentrios da Yoohyeon Eu estou no caminho para o trabalho Eu de repente me imaginei</t>
+          <t>Y pensar que ya no falta nada ksmdldllwe re rpido DreamcatcherndAlbum Apocalypse Saveus</t>
         </is>
       </c>
       <c r="F39" t="n">
         <v>0</v>
       </c>
       <c r="G39" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="H39" t="inlineStr">
         <is>
@@ -2038,7 +2038,7 @@
       </c>
       <c r="I39" t="inlineStr">
         <is>
-          <t>https://twitter.com/twitter/statuses/1513224785542754312</t>
+          <t>https://twitter.com/twitter/statuses/1513525485120069639</t>
         </is>
       </c>
     </row>
@@ -2050,7 +2050,7 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>adorn2u</t>
+          <t>SheaTheUnicorn</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
@@ -2059,11 +2059,11 @@
         </is>
       </c>
       <c r="D40" s="2" t="n">
-        <v>44662.06761574074</v>
+        <v>44662.89767361111</v>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>Excited to share this item from my etsy shop Charm Cages for Pearls Variety of Styles including</t>
+          <t>HOW AM I SUPPOSED TO SLEEP TONIGHTDreamcatcher Apocalypse ApocalypseSaveus hfdreamcatcher</t>
         </is>
       </c>
       <c r="F40" t="n">
@@ -2079,7 +2079,7 @@
       </c>
       <c r="I40" t="inlineStr">
         <is>
-          <t>https://twitter.com/twitter/statuses/1513224636053573648</t>
+          <t>https://twitter.com/twitter/statuses/1513525438500458502</t>
         </is>
       </c>
     </row>
@@ -2091,27 +2091,27 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>deukaemobile</t>
+          <t>bloodyponey</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>don't repost/claim as yours</t>
+          <t>21, she/her</t>
         </is>
       </c>
       <c r="D41" s="2" t="n">
-        <v>44662.06758101852</v>
+        <v>44662.89761574074</v>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>Maison 'MV Teaser' hfdreamcatcher Dreamcatcher ApocalypseSaveus MAISON</t>
+          <t>n usei as tags cedo to triste por isso vou usar agr DreamcatcherndAlbum Apocalypse Saveus MAISON</t>
         </is>
       </c>
       <c r="F41" t="n">
-        <v>77</v>
+        <v>0</v>
       </c>
       <c r="G41" t="n">
-        <v>288</v>
+        <v>0</v>
       </c>
       <c r="H41" t="inlineStr">
         <is>
@@ -2120,7 +2120,7 @@
       </c>
       <c r="I41" t="inlineStr">
         <is>
-          <t>https://twitter.com/twitter/statuses/1513224623437012993</t>
+          <t>https://twitter.com/twitter/statuses/1513525420716666890</t>
         </is>
       </c>
     </row>
@@ -2132,36 +2132,36 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>dc_stan_24024</t>
+          <t>DCSupportMX</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>unknown</t>
+          <t>For Dreamcatcher ♥︎</t>
         </is>
       </c>
       <c r="D42" s="2" t="n">
-        <v>44662.06744212963</v>
+        <v>44662.89761574074</v>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>Its past midnight in India right now and Im jamming to Dreamcatcher Playlist as if I dont have clg at 830 am tomorrow</t>
+          <t>TendenciaMAISON es Tendencia en Mxico Dreamcatcherhfdreamcatcher</t>
         </is>
       </c>
       <c r="F42" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G42" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>positive</t>
+          <t>neutral</t>
         </is>
       </c>
       <c r="I42" t="inlineStr">
         <is>
-          <t>https://twitter.com/twitter/statuses/1513224574464233474</t>
+          <t>https://twitter.com/twitter/statuses/1513525418883657733</t>
         </is>
       </c>
     </row>
@@ -2173,20 +2173,20 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>ellieofpeach</t>
+          <t>vidagris</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Canada</t>
+          <t>Rhode Island, USA</t>
         </is>
       </c>
       <c r="D43" s="2" t="n">
-        <v>44662.0668287037</v>
+        <v>44662.8975</v>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>dexter27aggs forkpopvote done Dreamcatcher DREAMCATCHERApocalypse ApocalypseSaveUs</t>
+          <t>Dreamcatcher InSomnia</t>
         </is>
       </c>
       <c r="F43" t="n">
@@ -2202,7 +2202,7 @@
       </c>
       <c r="I43" t="inlineStr">
         <is>
-          <t>https://twitter.com/twitter/statuses/1513224352933765126</t>
+          <t>https://twitter.com/twitter/statuses/1513525375598538757</t>
         </is>
       </c>
     </row>
@@ -2214,27 +2214,27 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>InSomnias_alarm</t>
+          <t>asiangirls_esp</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t xml:space="preserve">فعلوا جرس التنبيهات 🔔 </t>
+          <t>México</t>
         </is>
       </c>
       <c r="D44" s="2" t="n">
-        <v>44662.0652662037</v>
+        <v>44662.89702546296</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>M Countdown</t>
+          <t>TEASER DREAMCATCHER DREAMCATCHER 'Maison' Dance Previewhfdreamcatcher</t>
         </is>
       </c>
       <c r="F44" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G44" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="H44" t="inlineStr">
         <is>
@@ -2243,7 +2243,7 @@
       </c>
       <c r="I44" t="inlineStr">
         <is>
-          <t>https://twitter.com/twitter/statuses/1513223786522460168</t>
+          <t>https://twitter.com/twitter/statuses/1513525204005310469</t>
         </is>
       </c>
     </row>
@@ -2255,20 +2255,20 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Lunar1825</t>
+          <t>fn1yFulrzG8vFDG</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>unknown</t>
+          <t>대한민국</t>
         </is>
       </c>
       <c r="D45" s="2" t="n">
-        <v>44662.06509259259</v>
+        <v>44662.89693287037</v>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>LVale0703 jellyvotesph Done for Dreamcatcher ApocalypseSaveUs ApocalypseSaveus</t>
+          <t>This time the mv views album sales and music records will all break their own record Im not sure if well be</t>
         </is>
       </c>
       <c r="F45" t="n">
@@ -2279,12 +2279,12 @@
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>neutral</t>
+          <t>positive</t>
         </is>
       </c>
       <c r="I45" t="inlineStr">
         <is>
-          <t>https://twitter.com/twitter/statuses/1513223722446082051</t>
+          <t>https://twitter.com/twitter/statuses/1513525170170122240</t>
         </is>
       </c>
     </row>
@@ -2296,23 +2296,27 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>KomasJackc</t>
+          <t>kimsnaps</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>unknown</t>
+          <t>Venezuela</t>
         </is>
       </c>
       <c r="D46" s="2" t="n">
-        <v>44662.06451388889</v>
-      </c>
-      <c r="E46" t="inlineStr"/>
+        <v>44662.89666666667</v>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>Dreamcatcher 'What' MV 'PIRI' MV REACTION via YouTube Dreamcatcher hfdreamcatcher</t>
+        </is>
+      </c>
       <c r="F46" t="n">
         <v>0</v>
       </c>
       <c r="G46" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="H46" t="inlineStr">
         <is>
@@ -2321,7 +2325,7 @@
       </c>
       <c r="I46" t="inlineStr">
         <is>
-          <t>https://twitter.com/twitter/statuses/1513223515041902592</t>
+          <t>https://twitter.com/twitter/statuses/1513525075672285196</t>
         </is>
       </c>
     </row>
@@ -2333,20 +2337,20 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>DChaotic4</t>
+          <t>PhoenixRed</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Malaysia</t>
+          <t>Braavos</t>
         </is>
       </c>
       <c r="D47" s="2" t="n">
-        <v>44662.06172453704</v>
+        <v>44662.89577546297</v>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>singkkum looking forward to Sua No bot and Yoohyeon For ApocalypseSaveUsDREAMCATCHER</t>
+          <t>PS If you have support or information efforts for Dreamcatcher that you want to drop into this thread feel free</t>
         </is>
       </c>
       <c r="F47" t="n">
@@ -2357,12 +2361,12 @@
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>neutral</t>
+          <t>positive</t>
         </is>
       </c>
       <c r="I47" t="inlineStr">
         <is>
-          <t>https://twitter.com/twitter/statuses/1513222501328846851</t>
+          <t>https://twitter.com/twitter/statuses/1513524753977511936</t>
         </is>
       </c>
     </row>
@@ -2374,36 +2378,36 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Ray_DC07</t>
+          <t>PhoenixRed</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Dreamworld</t>
+          <t>Braavos</t>
         </is>
       </c>
       <c r="D48" s="2" t="n">
-        <v>44662.06092592593</v>
+        <v>44662.89577546297</v>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>Lets support this cause help promote and bring awareness of Global climate changes Let take a step forward and P</t>
+          <t>No matter how this comeback goes popularity or winswise my hope is that Dreamcatcher fans around the world can s</t>
         </is>
       </c>
       <c r="F48" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G48" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t>neutral</t>
+          <t>positive</t>
         </is>
       </c>
       <c r="I48" t="inlineStr">
         <is>
-          <t>https://twitter.com/twitter/statuses/1513222214241636352</t>
+          <t>https://twitter.com/twitter/statuses/1513524752270430212</t>
         </is>
       </c>
     </row>
@@ -2415,36 +2419,36 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>JiuDCStan17</t>
+          <t>PhoenixRed</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>unknown</t>
+          <t>Braavos</t>
         </is>
       </c>
       <c r="D49" s="2" t="n">
-        <v>44662.06054398148</v>
+        <v>44662.89577546297</v>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>so sexcApocalypseSaveUs MAISONDreamcatcher hfdreamcatcher</t>
+          <t>And finally a couple Dreamcatcher fan communities there are more these are the two I frequent</t>
         </is>
       </c>
       <c r="F49" t="n">
         <v>0</v>
       </c>
       <c r="G49" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t>neutral</t>
+          <t>positive</t>
         </is>
       </c>
       <c r="I49" t="inlineStr">
         <is>
-          <t>https://twitter.com/twitter/statuses/1513222074407395329</t>
+          <t>https://twitter.com/twitter/statuses/1513524750282285059</t>
         </is>
       </c>
     </row>
@@ -2456,27 +2460,27 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>JiuDCStan17</t>
+          <t>PhoenixRed</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>unknown</t>
+          <t>Braavos</t>
         </is>
       </c>
       <c r="D50" s="2" t="n">
-        <v>44662.05981481481</v>
+        <v>44662.89576388889</v>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>Tao po DCC Parestock naman daw po ApocalypseSaveUs MAISONDreamcatcher hfdreamcatcher</t>
+          <t>Heres some other accounts you may want to look at following if youre curious about what theyre doing to help</t>
         </is>
       </c>
       <c r="F50" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G50" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H50" t="inlineStr">
         <is>
@@ -2485,7 +2489,7 @@
       </c>
       <c r="I50" t="inlineStr">
         <is>
-          <t>https://twitter.com/twitter/statuses/1513221809654550528</t>
+          <t>https://twitter.com/twitter/statuses/1513524748604616709</t>
         </is>
       </c>
     </row>
@@ -2506,18 +2510,18 @@
         </is>
       </c>
       <c r="D51" s="2" t="n">
-        <v>44662.05858796297</v>
+        <v>44662.89576388889</v>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>Dreamcatcher fans were only a couple of days away from a new kpop album filled with group and solo content and</t>
+          <t>is a complete detailed guide on supporting Dreamcatcher no matter how much time or money</t>
         </is>
       </c>
       <c r="F51" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G51" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="H51" t="inlineStr">
         <is>
@@ -2526,7 +2530,7 @@
       </c>
       <c r="I51" t="inlineStr">
         <is>
-          <t>https://twitter.com/twitter/statuses/1513221367000408067</t>
+          <t>https://twitter.com/twitter/statuses/1513524746759065603</t>
         </is>
       </c>
     </row>
@@ -2538,27 +2542,27 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>dcatcherbr</t>
+          <t>PhoenixRed</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>Desde 05/12/2016</t>
+          <t>Braavos</t>
         </is>
       </c>
       <c r="D52" s="2" t="n">
-        <v>44662.0547337963</v>
+        <v>44662.89575231481</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>l VIDEO JiU com Somnias diante da rdio Young Street Andando para trs porque queria continu</t>
+          <t>is a microsite I created that provides a shortform guide to Dreamcatcher easy to pass t</t>
         </is>
       </c>
       <c r="F52" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="G52" t="n">
-        <v>28</v>
+        <v>1</v>
       </c>
       <c r="H52" t="inlineStr">
         <is>
@@ -2567,7 +2571,7 @@
       </c>
       <c r="I52" t="inlineStr">
         <is>
-          <t>https://twitter.com/twitter/statuses/1513219970427142146</t>
+          <t>https://twitter.com/twitter/statuses/1513524745064656898</t>
         </is>
       </c>
     </row>
@@ -2579,36 +2583,36 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>mellowgona1</t>
+          <t>minjiaremint</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>unknown</t>
+          <t>alone in the city</t>
         </is>
       </c>
       <c r="D53" s="2" t="n">
-        <v>44662.05427083333</v>
+        <v>44662.89575231481</v>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>My heart is pounding yall We are gonna get a whole lotta love from our girls in 1 day hfdreamcatcher</t>
+          <t>LuvDeukae DIAS PARA O APOCALYPSEDreamcatcher hfdreamcatcher</t>
         </is>
       </c>
       <c r="F53" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="G53" t="n">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="H53" t="inlineStr">
         <is>
-          <t>positive</t>
+          <t>neutral</t>
         </is>
       </c>
       <c r="I53" t="inlineStr">
         <is>
-          <t>https://twitter.com/twitter/statuses/1513219802965606400</t>
+          <t>https://twitter.com/twitter/statuses/1513524744338952198</t>
         </is>
       </c>
     </row>
@@ -2620,36 +2624,36 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>DCSupportMX</t>
+          <t>PhoenixRed</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>For Dreamcatcher ♥︎</t>
+          <t>Braavos</t>
         </is>
       </c>
       <c r="D54" s="2" t="n">
-        <v>44662.05400462963</v>
+        <v>44662.89575231481</v>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>Agotado 'Apocalypse Save Us' versin SLa Versin Limitada lleva un par de horas agotada en Ktownu Es</t>
+          <t>Dreamcatcher fans the comeback for new kpop 2nd Full Album Apocalypse Save Us is tomorrow Here is a thread o</t>
         </is>
       </c>
       <c r="F54" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G54" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="H54" t="inlineStr">
         <is>
-          <t>neutral</t>
+          <t>positive</t>
         </is>
       </c>
       <c r="I54" t="inlineStr">
         <is>
-          <t>https://twitter.com/twitter/statuses/1513219703442853889</t>
+          <t>https://twitter.com/twitter/statuses/1513524743395287040</t>
         </is>
       </c>
     </row>
@@ -2661,20 +2665,20 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>DChaotic4</t>
+          <t>StarlightAtiny7</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>Malaysia</t>
+          <t>Piratepopper only☠ stream link</t>
         </is>
       </c>
       <c r="D55" s="2" t="n">
-        <v>44662.05335648148</v>
+        <v>44662.89556712963</v>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>foryoohyeon looking forward to the live band sound outfit and choreo Solo song also what I really want to see h</t>
+          <t>SUA AND DAMIS ESPECIALLY IM SO EXCITED FOR DC 2ND ALBUM DREAMCATCHER</t>
         </is>
       </c>
       <c r="F55" t="n">
@@ -2685,12 +2689,12 @@
       </c>
       <c r="H55" t="inlineStr">
         <is>
-          <t>positive</t>
+          <t>neutral</t>
         </is>
       </c>
       <c r="I55" t="inlineStr">
         <is>
-          <t>https://twitter.com/twitter/statuses/1513219471476879361</t>
+          <t>https://twitter.com/twitter/statuses/1513524676257284102</t>
         </is>
       </c>
     </row>
@@ -2702,36 +2706,36 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>AkiyamaStore</t>
+          <t>jiubamisenpie</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>⏰ De Seg à Sab das 9h às 20h ⏰</t>
+          <t xml:space="preserve">SHE/HER </t>
         </is>
       </c>
       <c r="D56" s="2" t="n">
-        <v>44662.0503125</v>
+        <v>44662.89381944444</v>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>Hoje o ltimo dia para participar da CEG do Dreamcatcher Apocalypse Save us Ir ficar aberto at hQ</t>
+          <t>Spreading the world about global warming and warned everyone to save the earth Yes Dreamcatcher did it with a so</t>
         </is>
       </c>
       <c r="F56" t="n">
+        <v>2</v>
+      </c>
+      <c r="G56" t="n">
         <v>3</v>
       </c>
-      <c r="G56" t="n">
-        <v>6</v>
-      </c>
       <c r="H56" t="inlineStr">
         <is>
-          <t>neutral</t>
+          <t>positive</t>
         </is>
       </c>
       <c r="I56" t="inlineStr">
         <is>
-          <t>https://twitter.com/twitter/statuses/1513218366919651330</t>
+          <t>https://twitter.com/twitter/statuses/1513524044032720898</t>
         </is>
       </c>
     </row>
@@ -2743,20 +2747,20 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>killshx_t</t>
+          <t>StarlightAtiny7</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>17 | Any pronouns | ENTP</t>
+          <t>Piratepopper only☠ stream link</t>
         </is>
       </c>
       <c r="D57" s="2" t="n">
-        <v>44662.04884259259</v>
+        <v>44662.8925</v>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>I got the regular versions on hello82 and the limited edition on kpopusaonline this morning I took too long to pre</t>
+          <t>MADDOX COMPOSED TOGETHER TOOamp DREAMCATCHER</t>
         </is>
       </c>
       <c r="F57" t="n">
@@ -2767,12 +2771,12 @@
       </c>
       <c r="H57" t="inlineStr">
         <is>
-          <t>negative</t>
+          <t>neutral</t>
         </is>
       </c>
       <c r="I57" t="inlineStr">
         <is>
-          <t>https://twitter.com/twitter/statuses/1513217833504849923</t>
+          <t>https://twitter.com/twitter/statuses/1513523563965612034</t>
         </is>
       </c>
     </row>
@@ -2784,27 +2788,27 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>DCSupportMX</t>
+          <t>nathaneskin</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>For Dreamcatcher ♥︎</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="D58" s="2" t="n">
-        <v>44662.04724537037</v>
+        <v>44662.89201388889</v>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>SomniaMySomnies tiene este proyecto a partir del de Abril subir una foto con una plantita que sembre</t>
+          <t>H3IdolChamp Done for DREAMCATCHERdreamcatcher kpop grilsgroup jiu sua siyeon handong yoohyeon dami</t>
         </is>
       </c>
       <c r="F58" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G58" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="H58" t="inlineStr">
         <is>
@@ -2813,7 +2817,7 @@
       </c>
       <c r="I58" t="inlineStr">
         <is>
-          <t>https://twitter.com/twitter/statuses/1513217254384549888</t>
+          <t>https://twitter.com/twitter/statuses/1513523387481702403</t>
         </is>
       </c>
     </row>
@@ -2825,20 +2829,20 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>portalgahyeon</t>
+          <t>soulbennn</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>Brasil</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="D59" s="2" t="n">
-        <v>44662.04480324074</v>
+        <v>44662.89194444445</v>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>WEVERSE GAHYEON comentou o prprio post Estou indo dormir agora Boa noite a todos e j passou</t>
+          <t>Howwww sheee so cuteeDreamcatcher ApocalypseD1 hfdreamcatcher</t>
         </is>
       </c>
       <c r="F59" t="n">
@@ -2854,7 +2858,7 @@
       </c>
       <c r="I59" t="inlineStr">
         <is>
-          <t>https://twitter.com/twitter/statuses/1513216369885601797</t>
+          <t>https://twitter.com/twitter/statuses/1513523363494633473</t>
         </is>
       </c>
     </row>
@@ -2866,20 +2870,20 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>luvdongie</t>
+          <t>StarlightAtiny7</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>unknown</t>
+          <t>Piratepopper only☠ stream link</t>
         </is>
       </c>
       <c r="D60" s="2" t="n">
-        <v>44662.04408564815</v>
+        <v>44662.8915625</v>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>LVale0703 jellyvotesph done Dreamcatcher DreamcatcherComeback ApocalypseSaveUs</t>
+          <t>MAISON SOUNDING TOO GOODD DC ALWAYS PULL THRU LEEZ OLLOUNDER WE LOVE YOU DREAMCATCHER ApocalypseSaveUs</t>
         </is>
       </c>
       <c r="F60" t="n">
@@ -2890,12 +2894,12 @@
       </c>
       <c r="H60" t="inlineStr">
         <is>
-          <t>neutral</t>
+          <t>positive</t>
         </is>
       </c>
       <c r="I60" t="inlineStr">
         <is>
-          <t>https://twitter.com/twitter/statuses/1513216108916101124</t>
+          <t>https://twitter.com/twitter/statuses/1513523226315755521</t>
         </is>
       </c>
     </row>
@@ -2907,27 +2911,27 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>portalgahyeon</t>
+          <t>Muhamma93145096</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>Brasil</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="D61" s="2" t="n">
-        <v>44662.04387731481</v>
+        <v>44662.89144675926</v>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>WEVERSE Atualizao da GAHYEON no momentsAmo vocs amo vocs amo vocs Dreamcatcher</t>
+          <t>Did you know that Maison teaser only has 11 dislikes meanwhile the likes are 76KDreamcatcher 2ndAlbum</t>
         </is>
       </c>
       <c r="F61" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G61" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H61" t="inlineStr">
         <is>
@@ -2936,7 +2940,7 @@
       </c>
       <c r="I61" t="inlineStr">
         <is>
-          <t>https://twitter.com/twitter/statuses/1513216032814551045</t>
+          <t>https://twitter.com/twitter/statuses/1513523182615293952</t>
         </is>
       </c>
     </row>
@@ -2948,36 +2952,36 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>YoohyeonHourly</t>
+          <t>StarlightAtiny7</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>unknown</t>
+          <t>Piratepopper only☠ stream link</t>
         </is>
       </c>
       <c r="D62" s="2" t="n">
-        <v>44662.04166666666</v>
+        <v>44662.89079861111</v>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>Dreamcatcher YOOHYEON hfdreamcatcher</t>
+          <t>Maddox did lyrics for locked inside a door for dreamcatchers new comeback omggg Dreamcatcher ApocalypseSaveUs</t>
         </is>
       </c>
       <c r="F62" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G62" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="H62" t="inlineStr">
         <is>
-          <t>neutral</t>
+          <t>positive</t>
         </is>
       </c>
       <c r="I62" t="inlineStr">
         <is>
-          <t>https://twitter.com/twitter/statuses/1513215234709733377</t>
+          <t>https://twitter.com/twitter/statuses/1513522948455682060</t>
         </is>
       </c>
     </row>
@@ -2989,20 +2993,20 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>Dorothy20443918</t>
+          <t>MovoSaijari</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>unknown</t>
+          <t>Munchengladbach</t>
         </is>
       </c>
       <c r="D63" s="2" t="n">
-        <v>44662.04092592592</v>
+        <v>44662.89079861111</v>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>Dongie muscle so coolApocalypseSaveUs Dreamcatcher hfdreamcatcher</t>
+          <t>mymusictaste hfdreamcatcher dreamcatcherFaves Fave Dreamcatcher song SaharaFave Dreamcatcher MV BEcause</t>
         </is>
       </c>
       <c r="F63" t="n">
@@ -3018,7 +3022,7 @@
       </c>
       <c r="I63" t="inlineStr">
         <is>
-          <t>https://twitter.com/twitter/statuses/1513214964403638272</t>
+          <t>https://twitter.com/twitter/statuses/1513522947616653314</t>
         </is>
       </c>
     </row>
@@ -3030,27 +3034,27 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>DCSupportMX</t>
+          <t>MovoSaijari</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>For Dreamcatcher ♥︎</t>
+          <t>Munchengladbach</t>
         </is>
       </c>
       <c r="D64" s="2" t="n">
-        <v>44662.03966435185</v>
+        <v>44662.89075231482</v>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>GAHYEON WeverseLuv you luv you luv you Dreamcatcherhfdreamcatcher</t>
+          <t>mymusictaste hfdreamcatcher dreamcatcherFaves Fave Dreamcatcher song SaharaFave Dreamcatcher MV BEcause</t>
         </is>
       </c>
       <c r="F64" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G64" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H64" t="inlineStr">
         <is>
@@ -3059,7 +3063,7 @@
       </c>
       <c r="I64" t="inlineStr">
         <is>
-          <t>https://twitter.com/twitter/statuses/1513214507199336452</t>
+          <t>https://twitter.com/twitter/statuses/1513522929967017985</t>
         </is>
       </c>
     </row>
@@ -3071,20 +3075,20 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>perthiiz</t>
+          <t>MovoSaijari</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>unknown</t>
+          <t>Munchengladbach</t>
         </is>
       </c>
       <c r="D65" s="2" t="n">
-        <v>44662.0396412037</v>
+        <v>44662.89054398148</v>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>Dreamcatcher Heardle DreamcatcherndAlbumApocalypse Saveus</t>
+          <t>mymusictaste hfdreamcatcher dreamcatcherFaves Fave Dreamcatcher song SaharaFave Dreamcatcher MV BEcause</t>
         </is>
       </c>
       <c r="F65" t="n">
@@ -3100,7 +3104,7 @@
       </c>
       <c r="I65" t="inlineStr">
         <is>
-          <t>https://twitter.com/twitter/statuses/1513214501122097154</t>
+          <t>https://twitter.com/twitter/statuses/1513522857686573068</t>
         </is>
       </c>
     </row>
@@ -3112,27 +3116,27 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>dcatcherbr</t>
+          <t>MovoSaijari</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>Desde 05/12/2016</t>
+          <t>Munchengladbach</t>
         </is>
       </c>
       <c r="D66" s="2" t="n">
-        <v>44662.03809027778</v>
+        <v>44662.89049768518</v>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>l INFO SAHARA ultrapassou mil likes no MelOnDreamcatcher hfdreamcatcher</t>
+          <t>mymusictaste hfdreamcatcher dreamcatcherFaves Fave Dreamcatcher song SaharaFave Dreamcatcher MV BEcause</t>
         </is>
       </c>
       <c r="F66" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G66" t="n">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="H66" t="inlineStr">
         <is>
@@ -3141,7 +3145,7 @@
       </c>
       <c r="I66" t="inlineStr">
         <is>
-          <t>https://twitter.com/twitter/statuses/1513213937394884617</t>
+          <t>https://twitter.com/twitter/statuses/1513522837700714508</t>
         </is>
       </c>
     </row>
@@ -3153,20 +3157,20 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>skadolla</t>
+          <t>MovoSaijari</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>Dream's World</t>
+          <t>Munchengladbach</t>
         </is>
       </c>
       <c r="D67" s="2" t="n">
-        <v>44662.03579861111</v>
+        <v>44662.89018518518</v>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>Dreamcatcher Heardle 16 Dreamcatcher2ndAlbumApocalypse SaveusDreamcatcherComeback</t>
+          <t>mymusictaste hfdreamcatcher dreamcatcherFaves Fave Dreamcatcher song SaharaFave Dreamcatcher MV BEcause</t>
         </is>
       </c>
       <c r="F67" t="n">
@@ -3182,7 +3186,7 @@
       </c>
       <c r="I67" t="inlineStr">
         <is>
-          <t>https://twitter.com/twitter/statuses/1513213105110921216</t>
+          <t>https://twitter.com/twitter/statuses/1513522725209448448</t>
         </is>
       </c>
     </row>
@@ -3194,20 +3198,20 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>LUVPANDA_GG</t>
+          <t>MovoSaijari</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>unknown</t>
+          <t>Munchengladbach</t>
         </is>
       </c>
       <c r="D68" s="2" t="n">
-        <v>44662.03525462963</v>
+        <v>44662.89012731481</v>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>Dreamcatcher MAISON Teaser InSomnia MAISON Dreamcatcher Apocalypse Saveus</t>
+          <t>mymusictaste hfdreamcatcher dreamcatcherFaves Fave Dreamcatcher song SaharaFave Dreamcatcher MV BEcause</t>
         </is>
       </c>
       <c r="F68" t="n">
@@ -3223,7 +3227,7 @@
       </c>
       <c r="I68" t="inlineStr">
         <is>
-          <t>https://twitter.com/twitter/statuses/1513212908213350400</t>
+          <t>https://twitter.com/twitter/statuses/1513522704342790147</t>
         </is>
       </c>
     </row>
@@ -3235,27 +3239,27 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>hannahfrank115</t>
+          <t>i6_yubin</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>unknown</t>
+          <t xml:space="preserve">( . ) read the carrd 💭_ </t>
         </is>
       </c>
       <c r="D69" s="2" t="n">
-        <v>44662.0350925926</v>
+        <v>44662.89008101852</v>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>A piece of heaven bluelagoon iceland water nature dreamcatcher bucketlist paradiseonearth</t>
+          <t>LuvDeukae DIAS PARA O APOCALYPSEDreamcatcher hfdreamcatcher</t>
         </is>
       </c>
       <c r="F69" t="n">
         <v>0</v>
       </c>
       <c r="G69" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H69" t="inlineStr">
         <is>
@@ -3264,7 +3268,7 @@
       </c>
       <c r="I69" t="inlineStr">
         <is>
-          <t>https://twitter.com/twitter/statuses/1513212850902286337</t>
+          <t>https://twitter.com/twitter/statuses/1513522689989877766</t>
         </is>
       </c>
     </row>
@@ -3276,20 +3280,20 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>yoohsthetic</t>
+          <t>xiaopinktang</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>𖥔 ⭒ ִ ׂ 𝘀-𝗵𝗲𝗿! リトルバカ · ★☆</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="D70" s="2" t="n">
-        <v>44662.0344212963</v>
+        <v>44662.88987268518</v>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>foryoohyeon tysm for the ga im really looking forward to their title track maison 14SongsOfTheApocalypse</t>
+          <t>letgo DREAMCATCHER WJSN InSomniaXUjung DREAMCATCHERXWJSN</t>
         </is>
       </c>
       <c r="F70" t="n">
@@ -3305,7 +3309,7 @@
       </c>
       <c r="I70" t="inlineStr">
         <is>
-          <t>https://twitter.com/twitter/statuses/1513212605946470400</t>
+          <t>https://twitter.com/twitter/statuses/1513522613590507525</t>
         </is>
       </c>
     </row>
@@ -3317,27 +3321,27 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>toothless_eyes</t>
+          <t>MovoSaijari</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>Atiny Stay Moa Insomnia Tomoon</t>
+          <t>Munchengladbach</t>
         </is>
       </c>
       <c r="D71" s="2" t="n">
-        <v>44662.03381944444</v>
+        <v>44662.8897337963</v>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>TOMORROW Dreamcatcher ApocalypseSaveUs</t>
+          <t>mymusictaste hfdreamcatcher dreamcatcherFaves Fave Dreamcatcher song SaharaFave Dreamcatcher MV BEcause</t>
         </is>
       </c>
       <c r="F71" t="n">
         <v>0</v>
       </c>
       <c r="G71" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H71" t="inlineStr">
         <is>
@@ -3346,7 +3350,7 @@
       </c>
       <c r="I71" t="inlineStr">
         <is>
-          <t>https://twitter.com/twitter/statuses/1513212387796697097</t>
+          <t>https://twitter.com/twitter/statuses/1513522563837841409</t>
         </is>
       </c>
     </row>
@@ -3358,27 +3362,27 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>bluvitae7</t>
+          <t>DCSupportMX</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>she/her | 24</t>
+          <t>For Dreamcatcher ♥︎</t>
         </is>
       </c>
       <c r="D72" s="2" t="n">
-        <v>44662.03223379629</v>
+        <v>44662.88956018518</v>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>Dreamcatcher Heardle 15 Dreamcatcher2ndAlbumApocalypse SaveusDreamcatcherComeback</t>
+          <t>YouTube Streaming NO abran el vdeo en mltiples tabs NO le den refresh no adelanten no replay NO mute</t>
         </is>
       </c>
       <c r="F72" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G72" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H72" t="inlineStr">
         <is>
@@ -3387,7 +3391,7 @@
       </c>
       <c r="I72" t="inlineStr">
         <is>
-          <t>https://twitter.com/twitter/statuses/1513211816599601156</t>
+          <t>https://twitter.com/twitter/statuses/1513522498096181256</t>
         </is>
       </c>
     </row>
@@ -3399,7 +3403,7 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>yearlydeukae</t>
+          <t>soulbennn</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
@@ -3408,18 +3412,18 @@
         </is>
       </c>
       <c r="D73" s="2" t="n">
-        <v>44662.03125</v>
+        <v>44662.88947916667</v>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>Dreamcatcher JIU hfdreamcatcher</t>
+          <t>WowDreamcatcher ApocalypseD hfdreamcatcher</t>
         </is>
       </c>
       <c r="F73" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G73" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="H73" t="inlineStr">
         <is>
@@ -3428,7 +3432,7 @@
       </c>
       <c r="I73" t="inlineStr">
         <is>
-          <t>https://twitter.com/twitter/statuses/1513211457558614019</t>
+          <t>https://twitter.com/twitter/statuses/1513522470258884611</t>
         </is>
       </c>
     </row>
@@ -3440,27 +3444,27 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>yoohsthetic</t>
+          <t>lovedeukae</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>𖥔 ⭒ ִ ׂ 𝘀-𝗵𝗲𝗿! リトルバカ · ★☆</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="D74" s="2" t="n">
-        <v>44662.03003472222</v>
+        <v>44662.88938657408</v>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>singkkum tysm for the ga im really looking forward to suyoos solos 14SongsOfTheApocalypseApocalypseSaveUs Dreamcatcher</t>
+          <t>dongtasticnamu kmsvoting Done Dreamcatcher</t>
         </is>
       </c>
       <c r="F74" t="n">
         <v>0</v>
       </c>
       <c r="G74" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H74" t="inlineStr">
         <is>
@@ -3469,7 +3473,7 @@
       </c>
       <c r="I74" t="inlineStr">
         <is>
-          <t>https://twitter.com/twitter/statuses/1513211018259824641</t>
+          <t>https://twitter.com/twitter/statuses/1513522437555560448</t>
         </is>
       </c>
     </row>
@@ -3481,20 +3485,20 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>kimsnaps</t>
+          <t>saoroli</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>Venezuela</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="D75" s="2" t="n">
-        <v>44662.02921296296</v>
+        <v>44662.8887962963</v>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>The Bangers Dont Stop Dreamcatcher Odd Eye MV REACTION via YouTube</t>
+          <t>DeuKaeRadio TonyAguilarOfi Los GlobalShow hfdreamcatcher Hola TonyAguilarOfi Los GlobalShowNos</t>
         </is>
       </c>
       <c r="F75" t="n">
@@ -3505,12 +3509,12 @@
       </c>
       <c r="H75" t="inlineStr">
         <is>
-          <t>negative</t>
+          <t>neutral</t>
         </is>
       </c>
       <c r="I75" t="inlineStr">
         <is>
-          <t>https://twitter.com/twitter/statuses/1513210719629684750</t>
+          <t>https://twitter.com/twitter/statuses/1513522224577265683</t>
         </is>
       </c>
     </row>
@@ -3522,20 +3526,20 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>dreamcloud_mp3</t>
+          <t>inscape22</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>unknown</t>
+          <t>Miami, FL</t>
         </is>
       </c>
       <c r="D76" s="2" t="n">
-        <v>44662.0280324074</v>
+        <v>44662.88858796296</v>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>All that ambiance noise and Im just Dreamcatcher Heardle 15</t>
+          <t>Lets hope VOD will be made available later onDREAMCATCHER</t>
         </is>
       </c>
       <c r="F76" t="n">
@@ -3551,7 +3555,7 @@
       </c>
       <c r="I76" t="inlineStr">
         <is>
-          <t>https://twitter.com/twitter/statuses/1513210293534572548</t>
+          <t>https://twitter.com/twitter/statuses/1513522146345160711</t>
         </is>
       </c>
     </row>
@@ -3563,27 +3567,27 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>crowtitbora</t>
+          <t>kitsunejiu</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>急需娟雅狗糧</t>
+          <t>dee | 🇽🇰🇩🇪 | she/they/he</t>
         </is>
       </c>
       <c r="D77" s="2" t="n">
-        <v>44662.02690972222</v>
+        <v>44662.88765046297</v>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>Daily Siyeon tweetDreamcatcher Siyeon</t>
+          <t>Dreamcatcher Heardle 16 Dreamcatcher2ndAlbumApocalypse SaveusDreamcatcherComebackMAISON</t>
         </is>
       </c>
       <c r="F77" t="n">
         <v>0</v>
       </c>
       <c r="G77" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H77" t="inlineStr">
         <is>
@@ -3592,7 +3596,7 @@
       </c>
       <c r="I77" t="inlineStr">
         <is>
-          <t>https://twitter.com/twitter/statuses/1513209883910311937</t>
+          <t>https://twitter.com/twitter/statuses/1513521809752301577</t>
         </is>
       </c>
     </row>
@@ -3604,27 +3608,27 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>SuporteInsomnia</t>
+          <t>Cherry_Insomnia</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>unknown</t>
+          <t>대전 허리케인</t>
         </is>
       </c>
       <c r="D78" s="2" t="n">
-        <v>44662.02671296296</v>
+        <v>44662.88760416667</v>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>Lembrese de criar sua conta no site da MNET para poder votar no Dreamcatcher quando a votao do MCOUNTDOWN abrir</t>
+          <t>mymusictaste Dreamcatcher DREAMCATCHERFaves</t>
         </is>
       </c>
       <c r="F78" t="n">
-        <v>34</v>
+        <v>0</v>
       </c>
       <c r="G78" t="n">
-        <v>57</v>
+        <v>0</v>
       </c>
       <c r="H78" t="inlineStr">
         <is>
@@ -3633,7 +3637,7 @@
       </c>
       <c r="I78" t="inlineStr">
         <is>
-          <t>https://twitter.com/twitter/statuses/1513209812431028227</t>
+          <t>https://twitter.com/twitter/statuses/1513521793008795648</t>
         </is>
       </c>
     </row>
@@ -3645,36 +3649,36 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>dcatcherbr</t>
+          <t>_minpuppy_</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>Desde 05/12/2016</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="D79" s="2" t="n">
-        <v>44662.02622685185</v>
+        <v>44662.88653935185</v>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>l INSTAGRAM Atualizao da SuA no story sualelbora Clima agradvelDreamcatcher</t>
+          <t>People complain that in the new Dreamcatcher album there are no rock songsI mean they can try something differe</t>
         </is>
       </c>
       <c r="F79" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G79" t="n">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="H79" t="inlineStr">
         <is>
-          <t>neutral</t>
+          <t>negative</t>
         </is>
       </c>
       <c r="I79" t="inlineStr">
         <is>
-          <t>https://twitter.com/twitter/statuses/1513209637033725954</t>
+          <t>https://twitter.com/twitter/statuses/1513521406197350400</t>
         </is>
       </c>
     </row>
@@ -3686,27 +3690,27 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>crowtitbora</t>
+          <t>HrtBonny</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>急需娟雅狗糧</t>
+          <t>LOOΠΔVERSE</t>
         </is>
       </c>
       <c r="D80" s="2" t="n">
-        <v>44662.02592592593</v>
+        <v>44662.88585648148</v>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>Daily SuA tweetDreamcatcher SuA</t>
+          <t>ไปคะ พรุ่งนี้สาวๆคัมแบคแล้วว พร้อมฟาดด DreamcatcherndAlbum Apocalypse Saveus MAISON</t>
         </is>
       </c>
       <c r="F80" t="n">
         <v>0</v>
       </c>
       <c r="G80" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H80" t="inlineStr">
         <is>
@@ -3715,7 +3719,7 @@
       </c>
       <c r="I80" t="inlineStr">
         <is>
-          <t>https://twitter.com/twitter/statuses/1513209530116554752</t>
+          <t>https://twitter.com/twitter/statuses/1513521158884577282</t>
         </is>
       </c>
     </row>
@@ -3727,20 +3731,20 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>hoohoo126</t>
+          <t>sutarait0</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>trapped inside minnie's voice</t>
+          <t xml:space="preserve">RCBYF!! she/her. </t>
         </is>
       </c>
       <c r="D81" s="2" t="n">
-        <v>44662.02516203704</v>
+        <v>44662.88487268519</v>
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>my stan gg ranking 1 GIDLE 8 Apink27 Dreamcatcher</t>
+          <t>PaniclnTheCity hfdreamcatcher THANK YOU SO MUCH FOR THE GA hfdreamcatcher Dreamcatcher</t>
         </is>
       </c>
       <c r="F81" t="n">
@@ -3751,12 +3755,12 @@
       </c>
       <c r="H81" t="inlineStr">
         <is>
-          <t>negative</t>
+          <t>positive</t>
         </is>
       </c>
       <c r="I81" t="inlineStr">
         <is>
-          <t>https://twitter.com/twitter/statuses/1513209254194610177</t>
+          <t>https://twitter.com/twitter/statuses/1513520802959802368</t>
         </is>
       </c>
     </row>
@@ -3768,7 +3772,7 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>MJDC1STWIN</t>
+          <t>MaeMalielephan</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
@@ -3777,15 +3781,15 @@
         </is>
       </c>
       <c r="D82" s="2" t="n">
-        <v>44662.02297453704</v>
+        <v>44662.88445601852</v>
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>Thank youApocalypse Save Us hfdreamcatcher Dreamcatcher 14SongOfTheApocalypse</t>
+          <t>สวัสดีค่ะเมตตาเเม่มะลิได้นะค่ะDreamcatcher mixxiw เฌอสิค ข่าวใส่ไข่ ช้างตกงาน</t>
         </is>
       </c>
       <c r="F82" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G82" t="n">
         <v>0</v>
@@ -3797,7 +3801,7 @@
       </c>
       <c r="I82" t="inlineStr">
         <is>
-          <t>https://twitter.com/twitter/statuses/1513208460183490562</t>
+          <t>https://twitter.com/twitter/statuses/1513520651243425797</t>
         </is>
       </c>
     </row>
@@ -3809,36 +3813,36 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>StarlightDeukae</t>
+          <t>vampdami</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>US🇺🇸||Link about disability</t>
+          <t>she/they</t>
         </is>
       </c>
       <c r="D83" s="2" t="n">
-        <v>44662.02273148148</v>
+        <v>44662.88239583333</v>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>InSomnia the next and last drop before comeback day happens later Im so excited to see the dance preview</t>
+          <t>PaniclnTheCity hfdreamcatcher Thanks for the giveaway Good luck everyone Dreamcatcher</t>
         </is>
       </c>
       <c r="F83" t="n">
         <v>0</v>
       </c>
       <c r="G83" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H83" t="inlineStr">
         <is>
-          <t>neutral</t>
+          <t>positive</t>
         </is>
       </c>
       <c r="I83" t="inlineStr">
         <is>
-          <t>https://twitter.com/twitter/statuses/1513208371108884480</t>
+          <t>https://twitter.com/twitter/statuses/1513519903831113736</t>
         </is>
       </c>
     </row>
@@ -3850,20 +3854,20 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>saoroli</t>
+          <t>marin_lucu</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>unknown</t>
+          <t>Indonesia</t>
         </is>
       </c>
       <c r="D84" s="2" t="n">
-        <v>44662.02247685185</v>
+        <v>44662.88099537037</v>
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>LVale0703 jellyvotesph Done for Dreamcatcher Thanx so much somnie</t>
+          <t>DREAMCATCHER KTOWN4U LUCKY DRAW PROXYPrice 1922000Including proxy feeWith or without albumNo priorityI</t>
         </is>
       </c>
       <c r="F84" t="n">
@@ -3874,12 +3878,12 @@
       </c>
       <c r="H84" t="inlineStr">
         <is>
-          <t>positive</t>
+          <t>neutral</t>
         </is>
       </c>
       <c r="I84" t="inlineStr">
         <is>
-          <t>https://twitter.com/twitter/statuses/1513208278485979139</t>
+          <t>https://twitter.com/twitter/statuses/1513519397163651081</t>
         </is>
       </c>
     </row>
@@ -3891,20 +3895,20 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>NordskovSomnia</t>
+          <t>risa_somnia</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>Spain • She/her • Esp/Eng</t>
+          <t>The Dream World</t>
         </is>
       </c>
       <c r="D85" s="2" t="n">
-        <v>44662.02121527777</v>
+        <v>44662.88042824074</v>
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>DreamCatcher hfdreamcatcher</t>
+          <t>Just preordered all 4 albums RIP to my Canadian walletDreamcatcher ApocalypseSaveUs</t>
         </is>
       </c>
       <c r="F85" t="n">
@@ -3920,7 +3924,7 @@
       </c>
       <c r="I85" t="inlineStr">
         <is>
-          <t>https://twitter.com/twitter/statuses/1513207820556156939</t>
+          <t>https://twitter.com/twitter/statuses/1513519188622692360</t>
         </is>
       </c>
     </row>
@@ -3932,27 +3936,27 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>yoohsthetic</t>
+          <t>JUSTSINGJI</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>𖥔 ⭒ ִ ׂ 𝘀-𝗵𝗲𝗿! リトルバカ · ★☆</t>
+          <t>🐰🐺 ♡ JIU SIYEON</t>
         </is>
       </c>
       <c r="D86" s="2" t="n">
-        <v>44662.02068287037</v>
+        <v>44662.88013888889</v>
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>symylife tysm for the ga id like the S ver 14SongsOfTheApocalypseApocalypseSaveUs Dreamcatcher</t>
+          <t>DREAMCATCHER JIU SIYEONDREAMCATCHERApocalypse</t>
         </is>
       </c>
       <c r="F86" t="n">
         <v>0</v>
       </c>
       <c r="G86" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H86" t="inlineStr">
         <is>
@@ -3961,7 +3965,7 @@
       </c>
       <c r="I86" t="inlineStr">
         <is>
-          <t>https://twitter.com/twitter/statuses/1513207630654689280</t>
+          <t>https://twitter.com/twitter/statuses/1513519084763480065</t>
         </is>
       </c>
     </row>
@@ -3973,20 +3977,20 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>thvigoo</t>
+          <t>Kimsheesh_kpop</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>25</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="D87" s="2" t="n">
-        <v>44662.01886574074</v>
+        <v>44662.87980324074</v>
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>deukaeKdata thanks for the giveaway wish me luck ApocalypseSaveUs Dreamcatcher</t>
+          <t>Most Viewed Dreamcatcher Video of the past 7 Days 1 Boca 638k 2 2nd Album Highlight Medley 428k3 BEcause 36</t>
         </is>
       </c>
       <c r="F87" t="n">
@@ -3997,12 +4001,12 @@
       </c>
       <c r="H87" t="inlineStr">
         <is>
-          <t>neutral</t>
+          <t>negative</t>
         </is>
       </c>
       <c r="I87" t="inlineStr">
         <is>
-          <t>https://twitter.com/twitter/statuses/1513206968911273989</t>
+          <t>https://twitter.com/twitter/statuses/1513518966093791240</t>
         </is>
       </c>
     </row>
@@ -4014,36 +4018,36 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>CoalSolution</t>
+          <t>MerokoLady</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>unknown</t>
+          <t>she / her</t>
         </is>
       </c>
       <c r="D88" s="2" t="n">
-        <v>44662.01804398148</v>
+        <v>44662.87957175926</v>
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>7DREAMERS 220411 Gahyeon Weverse Moment commentGH Im going to sleep now Sleep well everyone its past mid</t>
+          <t>listen we WILL get this damned first win i will not sit here and watch another comeback go by without oneive</t>
         </is>
       </c>
       <c r="F88" t="n">
         <v>0</v>
       </c>
       <c r="G88" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H88" t="inlineStr">
         <is>
-          <t>negative</t>
+          <t>positive</t>
         </is>
       </c>
       <c r="I88" t="inlineStr">
         <is>
-          <t>https://twitter.com/twitter/statuses/1513206670922559502</t>
+          <t>https://twitter.com/twitter/statuses/1513518879250817028</t>
         </is>
       </c>
     </row>
@@ -4055,27 +4059,27 @@
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>palewavessss</t>
+          <t>Genevieve_Yoso</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>unknown</t>
+          <t>Watching from my Shrine</t>
         </is>
       </c>
       <c r="D89" s="2" t="n">
-        <v>44662.01767361111</v>
+        <v>44662.87922453704</v>
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>foryoohyeon the personality of each of them in a song DREAMCATCHER DREAMCATCHERApocalypse</t>
+          <t>EY HAVE YALL SEEN THE DANCE PREVIEW YET MAISON GONNA BE AMAZING Dreamcatcher</t>
         </is>
       </c>
       <c r="F89" t="n">
         <v>0</v>
       </c>
       <c r="G89" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H89" t="inlineStr">
         <is>
@@ -4084,7 +4088,7 @@
       </c>
       <c r="I89" t="inlineStr">
         <is>
-          <t>https://twitter.com/twitter/statuses/1513206538659270659</t>
+          <t>https://twitter.com/twitter/statuses/1513518752775684103</t>
         </is>
       </c>
     </row>
@@ -4096,27 +4100,27 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>ewexyoo</t>
+          <t>DCSupportMX</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>unknown</t>
+          <t>For Dreamcatcher ♥︎</t>
         </is>
       </c>
       <c r="D90" s="2" t="n">
-        <v>44662.01648148148</v>
+        <v>44662.87893518519</v>
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>foryoohyeon DREAMCATCHERApocalypse Dreamcatcher</t>
+          <t>GMAHallypop DeuKaeRadio hfdreamcatcher Dami DreamcatcherApocalypseSaveUs</t>
         </is>
       </c>
       <c r="F90" t="n">
         <v>0</v>
       </c>
       <c r="G90" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H90" t="inlineStr">
         <is>
@@ -4125,7 +4129,7 @@
       </c>
       <c r="I90" t="inlineStr">
         <is>
-          <t>https://twitter.com/twitter/statuses/1513206105257742343</t>
+          <t>https://twitter.com/twitter/statuses/1513518649163747330</t>
         </is>
       </c>
     </row>
@@ -4137,27 +4141,27 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>dcatcherbr</t>
+          <t>SeptemCalendis</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>Desde 05/12/2016</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="D91" s="2" t="n">
-        <v>44662.01532407408</v>
+        <v>44662.87769675926</v>
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>l WEVERSE Comentrio da HandongF Unnie voc pode fechar os olhos e escrever o nome das membros Kek</t>
+          <t>WEVERSE Duerman bien y nos vemos maana jeje YOOHYEON Dreamcatcher hfdreamcatcher</t>
         </is>
       </c>
       <c r="F91" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G91" t="n">
-        <v>27</v>
+        <v>0</v>
       </c>
       <c r="H91" t="inlineStr">
         <is>
@@ -4166,7 +4170,7 @@
       </c>
       <c r="I91" t="inlineStr">
         <is>
-          <t>https://twitter.com/twitter/statuses/1513205687966441482</t>
+          <t>https://twitter.com/twitter/statuses/1513518199656095755</t>
         </is>
       </c>
     </row>
@@ -4178,27 +4182,27 @@
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>toDC170113</t>
+          <t>DCSupportMX</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>unknown</t>
+          <t>For Dreamcatcher ♥︎</t>
         </is>
       </c>
       <c r="D92" s="2" t="n">
-        <v>44662.01327546296</v>
+        <v>44662.87699074074</v>
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t>About music shows and their scoring system410There are some changes M Countdownvoting system 47 scor</t>
+          <t>DeuKaeRadio TonyAguilarOfi Los GlobalShow hfdreamcatcher TonyAguilarOfi Los GlobalShow Hola Nos</t>
         </is>
       </c>
       <c r="F92" t="n">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="G92" t="n">
-        <v>42</v>
+        <v>0</v>
       </c>
       <c r="H92" t="inlineStr">
         <is>
@@ -4207,7 +4211,7 @@
       </c>
       <c r="I92" t="inlineStr">
         <is>
-          <t>https://twitter.com/twitter/statuses/1513204944484339713</t>
+          <t>https://twitter.com/twitter/statuses/1513517944558403588</t>
         </is>
       </c>
     </row>
@@ -4219,27 +4223,27 @@
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>Arab_Insomnias</t>
+          <t>xllii_li8</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>التغطية في الإعجابات ♥️</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="D93" s="2" t="n">
-        <v>44662.01318287037</v>
+        <v>44662.87670138889</v>
       </c>
       <c r="E93" t="inlineStr">
         <is>
-          <t>Apocalypse Save Us Ktownu</t>
+          <t>Dreamcatcher</t>
         </is>
       </c>
       <c r="F93" t="n">
         <v>0</v>
       </c>
       <c r="G93" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="H93" t="inlineStr">
         <is>
@@ -4248,7 +4252,7 @@
       </c>
       <c r="I93" t="inlineStr">
         <is>
-          <t>https://twitter.com/twitter/statuses/1513204910363402247</t>
+          <t>https://twitter.com/twitter/statuses/1513517837922582534</t>
         </is>
       </c>
     </row>
@@ -4260,27 +4264,27 @@
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>iomisonoperso</t>
+          <t>0lddami</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>Parma / Earth / Solar System</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="D94" s="2" t="n">
-        <v>44662.01266203704</v>
+        <v>44662.87663194445</v>
       </c>
       <c r="E94" t="inlineStr">
         <is>
-          <t>There is no passivity in the night Non c' passivit nella notteReadings about night and dreams</t>
+          <t>dongtasticnamu kmsvoting done for dreamcatcher lt3</t>
         </is>
       </c>
       <c r="F94" t="n">
         <v>0</v>
       </c>
       <c r="G94" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H94" t="inlineStr">
         <is>
@@ -4289,7 +4293,7 @@
       </c>
       <c r="I94" t="inlineStr">
         <is>
-          <t>https://twitter.com/twitter/statuses/1513204724203507713</t>
+          <t>https://twitter.com/twitter/statuses/1513517815256469507</t>
         </is>
       </c>
     </row>
@@ -4301,20 +4305,20 @@
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>PKorea2U</t>
+          <t>aoi_philip</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>Check Status Click Link</t>
+          <t>Piracicaba, Brasil</t>
         </is>
       </c>
       <c r="D95" s="2" t="n">
-        <v>44662.01177083333</v>
+        <v>44662.87662037037</v>
       </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t>ปิดพรีวันนี้แล้วนะคะ สิบโมงเช้า สอมเนียอย่าลืมสั่งน้าาDreamcatcher Apocalypse Save us S AVE</t>
+          <t>npomvtt Espero que no tenham anunciado o policial para fazer suspense ele precisa estar vivo DIA PARA O APO</t>
         </is>
       </c>
       <c r="F95" t="n">
@@ -4330,7 +4334,7 @@
       </c>
       <c r="I95" t="inlineStr">
         <is>
-          <t>https://twitter.com/twitter/statuses/1513204399824244736</t>
+          <t>https://twitter.com/twitter/statuses/1513517812593139720</t>
         </is>
       </c>
     </row>
@@ -4342,7 +4346,7 @@
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>toDC170113</t>
+          <t>SeptemCalendis</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
@@ -4351,18 +4355,18 @@
         </is>
       </c>
       <c r="D96" s="2" t="n">
-        <v>44662.00828703704</v>
+        <v>44662.87637731482</v>
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t>Dreamcatcher DreamcatcherComeback hfdreamcatcher</t>
+          <t>WEVERSE Teamoteamoteamo GAHYEON Dreamcatcher hfdreamcatcher</t>
         </is>
       </c>
       <c r="F96" t="n">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="G96" t="n">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="H96" t="inlineStr">
         <is>
@@ -4371,7 +4375,7 @@
       </c>
       <c r="I96" t="inlineStr">
         <is>
-          <t>https://twitter.com/twitter/statuses/1513203137141964803</t>
+          <t>https://twitter.com/twitter/statuses/1513517720784023553</t>
         </is>
       </c>
     </row>
@@ -4383,27 +4387,27 @@
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>JTP_KPOP</t>
+          <t>DChaotic4</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>JTP ENTERTAINMENT</t>
+          <t>Malaysia</t>
         </is>
       </c>
       <c r="D97" s="2" t="n">
-        <v>44662.00815972222</v>
+        <v>44662.87604166667</v>
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t>Dreamcatcher 'MAISON' MV Teaser</t>
+          <t>NooBabyNoo TYSM for the GA hfdreamcatcher2ndAlbum DreamcatcherApocalypseSaveUs</t>
         </is>
       </c>
       <c r="F97" t="n">
         <v>0</v>
       </c>
       <c r="G97" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H97" t="inlineStr">
         <is>
@@ -4412,7 +4416,7 @@
       </c>
       <c r="I97" t="inlineStr">
         <is>
-          <t>https://twitter.com/twitter/statuses/1513203091226918913</t>
+          <t>https://twitter.com/twitter/statuses/1513517602131562501</t>
         </is>
       </c>
     </row>
@@ -4424,7 +4428,7 @@
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>conundrum329</t>
+          <t>SeptemCalendis</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
@@ -4433,11 +4437,11 @@
         </is>
       </c>
       <c r="D98" s="2" t="n">
-        <v>44662.00703703704</v>
+        <v>44662.87604166667</v>
       </c>
       <c r="E98" t="inlineStr">
         <is>
-          <t>quote night Dreamcatcher life</t>
+          <t>WEVERSE Me prob el sombrero de YootonieEs esta la forma correcta DAMI Dreamcatcher</t>
         </is>
       </c>
       <c r="F98" t="n">
@@ -4453,7 +4457,7 @@
       </c>
       <c r="I98" t="inlineStr">
         <is>
-          <t>https://twitter.com/twitter/statuses/1513202685117603840</t>
+          <t>https://twitter.com/twitter/statuses/1513517601917386761</t>
         </is>
       </c>
     </row>
@@ -4465,36 +4469,36 @@
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>mellowgona1</t>
+          <t>Dreamcatcher_ir</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>unknown</t>
+          <t>اولین فن بیس فارسی دریم کچر</t>
         </is>
       </c>
       <c r="D99" s="2" t="n">
-        <v>44662.00609953704</v>
+        <v>44662.87591435185</v>
       </c>
       <c r="E99" t="inlineStr">
         <is>
-          <t>Flat earthers are claiming this was staged and this never happened What you all say guys hfdreamcatcher</t>
+          <t>My Music Taste Apocalypse Save us</t>
         </is>
       </c>
       <c r="F99" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G99" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="H99" t="inlineStr">
         <is>
-          <t>negative</t>
+          <t>neutral</t>
         </is>
       </c>
       <c r="I99" t="inlineStr">
         <is>
-          <t>https://twitter.com/twitter/statuses/1513202345378979842</t>
+          <t>https://twitter.com/twitter/statuses/1513517554916077581</t>
         </is>
       </c>
     </row>
@@ -4506,27 +4510,27 @@
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>caramelcream_MY</t>
+          <t>HANDONGmybias</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t xml:space="preserve">Dream World </t>
+          <t>No, Yoohyeon is my bias</t>
         </is>
       </c>
       <c r="D100" s="2" t="n">
-        <v>44662.00454861111</v>
+        <v>44662.87541666667</v>
       </c>
       <c r="E100" t="inlineStr">
         <is>
-          <t>hfdreamcatcher Dreamcatcher ApocalypseSaveUs</t>
+          <t>PaniclnTheCity hfdreamcatcher Thank you for the GA hfdreamcatcher Dreamcatcher MAISON</t>
         </is>
       </c>
       <c r="F100" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G100" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H100" t="inlineStr">
         <is>
@@ -4535,7 +4539,7 @@
       </c>
       <c r="I100" t="inlineStr">
         <is>
-          <t>https://twitter.com/twitter/statuses/1513201783895891969</t>
+          <t>https://twitter.com/twitter/statuses/1513517375974432770</t>
         </is>
       </c>
     </row>
@@ -4547,27 +4551,27 @@
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>dcatcherbr</t>
+          <t>SeptemCalendis</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>Desde 05/12/2016</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="D101" s="2" t="n">
-        <v>44662.00418981481</v>
+        <v>44662.8753125</v>
       </c>
       <c r="E101" t="inlineStr">
         <is>
-          <t>l VIDEO JiU com Somnias diante da rdio Young Street Eu farei o meu melhor e voltar Obri</t>
+          <t>WEVERSE Mis amoresPor favor anticipen mucho JIU Dreamcatcher hfdreamcatcher</t>
         </is>
       </c>
       <c r="F101" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G101" t="n">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="H101" t="inlineStr">
         <is>
@@ -4576,7 +4580,7 @@
       </c>
       <c r="I101" t="inlineStr">
         <is>
-          <t>https://twitter.com/twitter/statuses/1513201653515706368</t>
+          <t>https://twitter.com/twitter/statuses/1513517334920638464</t>
         </is>
       </c>
     </row>

</xml_diff>